<commit_message>
Added ability to parse worksheet with errors
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2040" windowWidth="23040" windowHeight="9564"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="23040" windowHeight="9564" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -353,7 +354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -49600,4 +49601,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="e">
+        <f>10/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B1" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C1" t="e">
+        <f>MONTH(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D1" t="e">
+        <f>MONTH("string")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test for custom format parsing
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkennell\Projects\xlsxir\test\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennell/Projects/elixir/xlsxir Library/xlsxir/test/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="23040" windowHeight="9564" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -40,6 +44,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="4">
+    <numFmt numFmtId="171" formatCode="\_x0009_\ ####.#"/>
+    <numFmt numFmtId="173" formatCode="#.0#"/>
+    <numFmt numFmtId="174" formatCode="yyyy"/>
+    <numFmt numFmtId="175" formatCode="mmm/dd/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,9 +79,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,9 +149,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -170,9 +184,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -358,9 +372,9 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,9 +405,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -401,7 +415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -422,9 +436,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -49591,9 +49605,9 @@
       <selection activeCell="B1048576" sqref="B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1048576" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1048576">
         <v>1048576</v>
       </c>
@@ -49607,13 +49621,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="e">
         <f>10/0</f>
         <v>#DIV/0!</v>
@@ -49629,6 +49643,35 @@
       <c r="D1" t="e">
         <f>MONTH("string")</f>
         <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>-123.45</v>
+      </c>
+      <c r="B1" s="3">
+        <v>67.89</v>
+      </c>
+      <c r="C1" s="4">
+        <v>42005</v>
+      </c>
+      <c r="D1" s="5">
+        <v>42735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes #27 - Conditional formatting
- Looking into this a bit more, the issue seems to be that
  ParseWorksheet expects to never hit another match of
  `sax_parse_event({:character...` following the last
  row of data.  Adjusted the parser to instead return the
  existing state object as the return for the end of the row
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennell/Projects/elixir/xlsxir Library/xlsxir/test/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinn/Development/elixir/xlsxir/test/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,13 @@
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>string one</t>
   </si>
   <si>
     <t>string two</t>
+  </si>
+  <si>
+    <t>Conditional</t>
   </si>
 </sst>
 </file>
@@ -45,15 +52,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="171" formatCode="\_x0009_\ ####.#"/>
-    <numFmt numFmtId="173" formatCode="#.0#"/>
-    <numFmt numFmtId="174" formatCode="yyyy"/>
-    <numFmt numFmtId="175" formatCode="mmm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="\_x0009_\ ####.#"/>
+    <numFmt numFmtId="165" formatCode="#.0#"/>
+    <numFmt numFmtId="166" formatCode="yyyy"/>
+    <numFmt numFmtId="167" formatCode="mmm/dd/yyyy"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,18 +93,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -49654,7 +49690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -49677,4 +49713,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Conditional"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for parsing cells with boolean values
Added tests
Added sheet8 in test/test_data/test.xlsx having truthy values
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinn/Development/elixir/xlsxir/test/test_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,16 +14,17 @@
     <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -105,17 +101,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -182,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -217,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -394,7 +380,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,9 +394,9 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,6 +416,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -441,9 +432,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -451,7 +442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -461,6 +452,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -472,9 +468,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16384">
       <c r="A1">
         <v>1</v>
       </c>
@@ -49630,6 +49626,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -49641,15 +49642,20 @@
       <selection activeCell="B1048576" sqref="B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1048576" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1048576" spans="1:1">
       <c r="A1048576">
         <v>1048576</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -49661,9 +49667,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="e">
         <f>10/0</f>
         <v>#DIV/0!</v>
@@ -49683,6 +49689,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -49694,9 +49705,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2">
         <v>-123.45</v>
       </c>
@@ -49712,6 +49723,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -49719,26 +49735,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for parsing time values
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -1,44 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
+  <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="7"/>
+    <workbookView activeTab="5" windowWidth="12800" windowHeight="4410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sheet2"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet3"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"Sheet4"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="4">"Sheet5"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="5">"Sheet6"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="6">"Sheet7"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="7">"Sheet8"</definedName>
+  </definedNames>
+  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
+  <webPublishing allowPng="1" css="0" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>string one</t>
-  </si>
-  <si>
-    <t>string two</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
   <si>
     <t>Conditional</t>
   </si>
@@ -46,27 +48,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="\_x0009_\ ####.#"/>
-    <numFmt numFmtId="165" formatCode="#.0#"/>
-    <numFmt numFmtId="166" formatCode="yyyy"/>
-    <numFmt numFmtId="167" formatCode="mmm/dd/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt formatCode="\_x0009_\ ####.#" numFmtId="100"/>
+    <numFmt formatCode="#.0#" numFmtId="101"/>
+    <numFmt formatCode="yyyy" numFmtId="102"/>
+    <numFmt formatCode="mmm/dd/yyyy" numFmtId="103"/>
+    <numFmt formatCode="[$-80A]hh:mm:ss\ AM/PM;@" numFmtId="104"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="0"/>
+      <i val="0"/>
+      <u val="none"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
+      <vertAlign val="baseline"/>
+      <sz val="10"/>
+      <strike val="0"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b val="0"/>
+      <i val="0"/>
+      <u val="none"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <vertAlign val="baseline"/>
+      <sz val="11"/>
+      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,330 +87,96 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+    <border diagonalUp="0" diagonalDown="0">
+      <left style="none">
+        <color rgb="FFC7C7C7"/>
+      </left>
+      <right style="none">
+        <color rgb="FFC7C7C7"/>
+      </right>
+      <top style="none">
+        <color rgb="FFC7C7C7"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+  <cellXfs count="9">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="14" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="101" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="102" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="103" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="104" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
   <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>string one</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>string two</t>
+        </is>
       </c>
       <c r="C1">
         <v>10</v>
@@ -410,29 +185,37 @@
         <f>4*5</f>
         <v>20</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="2">
         <v>42370</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
@@ -451,24 +234,32 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:XFD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16384">
       <c r="A1">
@@ -49625,24 +49416,32 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1048576" sqref="B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+  </cols>
   <sheetData>
     <row r="1048576" spans="1:1">
       <c r="A1048576">
@@ -49650,24 +49449,32 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="e">
@@ -49688,91 +49495,118 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="4" style="1" width="9.142307692307693"/>
+    <col min="5" max="5" style="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" style="1" width="9.142307692307693"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2">
+    <row r="1" spans="1:5">
+      <c r="A1" s="3">
         <v>-123.45</v>
       </c>
-      <c r="B1" s="3">
-        <v>67.89</v>
-      </c>
-      <c r="C1" s="4">
+      <c r="B1" s="4">
+        <v>67.890000000000001</v>
+      </c>
+      <c r="C1" s="5">
         <v>42005</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="6">
         <v>42735</v>
+      </c>
+      <c r="E1" s="7">
+        <v>0.63385416666666672</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" style="1" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="6" t="s">
-        <v>2</v>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.1"/>
+  <cols>
+    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="b">
@@ -49783,11 +49617,13 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added dependency to Timex for datetime shifts, modified test xlsx file and validated that all tests pass
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="5" windowWidth="12800" windowHeight="4410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="4410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,31 +18,37 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sheet2"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet3"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="3">"Sheet4"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="4">"Sheet5"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="5">"Sheet6"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="6">"Sheet7"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="7">"Sheet8"</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="125725"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Conditional</t>
+  </si>
+  <si>
+    <t>string one</t>
+  </si>
+  <si>
+    <t>string two</t>
   </si>
 </sst>
 </file>
@@ -50,32 +56,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt formatCode="\_x0009_\ ####.#" numFmtId="100"/>
-    <numFmt formatCode="#.0#" numFmtId="101"/>
-    <numFmt formatCode="yyyy" numFmtId="102"/>
-    <numFmt formatCode="mmm/dd/yyyy" numFmtId="103"/>
-    <numFmt formatCode="[$-80A]hh:mm:ss\ AM/PM;@" numFmtId="104"/>
+    <numFmt numFmtId="164" formatCode="\_x0009_\ ####.#"/>
+    <numFmt numFmtId="165" formatCode="#.0#"/>
+    <numFmt numFmtId="166" formatCode="yyyy"/>
+    <numFmt numFmtId="167" formatCode="mmm/dd/yyyy"/>
+    <numFmt numFmtId="168" formatCode="[$-80A]hh:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <vertAlign val="baseline"/>
-      <sz val="11"/>
-      <strike val="0"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,55 +84,32 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="14" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="101" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="102" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="103" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="104" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
   <dxfs count="1">
     <dxf>
       <font>
@@ -148,35 +122,310 @@
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>string one</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>string two</t>
-        </is>
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
       </c>
       <c r="C1">
         <v>10</v>
@@ -191,9 +440,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -202,19 +450,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -235,9 +480,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -246,19 +490,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -49417,9 +49658,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -49428,19 +49668,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1048576" sqref="B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1048576" spans="1:1">
@@ -49450,9 +49687,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -49461,19 +49697,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -49496,9 +49729,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -49507,29 +49739,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" style="1" width="9.142307692307693"/>
-    <col min="5" max="5" style="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="3">
         <v>-123.45</v>
       </c>
       <c r="B1" s="4">
-        <v>67.890000000000001</v>
+        <v>67.89</v>
       </c>
       <c r="C1" s="5">
         <v>42005</v>
@@ -49539,13 +49770,15 @@
       </c>
       <c r="E1" s="7">
         <v>0.63385416666666672</v>
+      </c>
+      <c r="F1" s="9">
+        <v>41261.601388888899</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -49554,20 +49787,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -49582,9 +49812,8 @@
       <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -49593,19 +49822,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -49618,9 +49844,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
added a peek() option and a related test
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="4410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="4410" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Conditional</t>
   </si>
@@ -49,6 +50,66 @@
   </si>
   <si>
     <t>string two</t>
+  </si>
+  <si>
+    <t>Col1</t>
+  </si>
+  <si>
+    <t>Col2</t>
+  </si>
+  <si>
+    <t>Col3</t>
+  </si>
+  <si>
+    <t>Col4</t>
+  </si>
+  <si>
+    <t>Col5</t>
+  </si>
+  <si>
+    <t>Col6</t>
+  </si>
+  <si>
+    <t>Col7</t>
+  </si>
+  <si>
+    <t>Col8</t>
+  </si>
+  <si>
+    <t>Col9</t>
+  </si>
+  <si>
+    <t>Col10</t>
+  </si>
+  <si>
+    <t>Col11</t>
+  </si>
+  <si>
+    <t>Col12</t>
+  </si>
+  <si>
+    <t>Col13</t>
+  </si>
+  <si>
+    <t>Col14</t>
+  </si>
+  <si>
+    <t>Col15</t>
+  </si>
+  <si>
+    <t>Some</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Interspersed</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -62,7 +123,7 @@
     <numFmt numFmtId="167" formatCode="mmm/dd/yyyy"/>
     <numFmt numFmtId="168" formatCode="[$-80A]hh:mm:ss\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -73,6 +134,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -106,6 +174,18 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -49851,4 +49931,3075 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="14" width="9.140625" style="10"/>
+    <col min="15" max="15" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10">
+        <v>4</v>
+      </c>
+      <c r="E2" s="10">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10">
+        <v>6</v>
+      </c>
+      <c r="G2" s="10">
+        <v>7</v>
+      </c>
+      <c r="H2" s="10">
+        <v>8</v>
+      </c>
+      <c r="I2" s="10">
+        <v>9</v>
+      </c>
+      <c r="J2" s="10">
+        <v>10</v>
+      </c>
+      <c r="K2" s="10">
+        <v>11</v>
+      </c>
+      <c r="L2" s="10">
+        <v>12</v>
+      </c>
+      <c r="M2" s="10">
+        <v>13</v>
+      </c>
+      <c r="N2" s="10">
+        <v>14</v>
+      </c>
+      <c r="O2" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <f>B2+A3</f>
+        <v>4</v>
+      </c>
+      <c r="C3" s="10">
+        <f t="shared" ref="C3:O3" si="0">C2+B3</f>
+        <v>7</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F3" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="I3" s="10">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="J3" s="10">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="K3" s="10">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="L3" s="10">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="M3" s="10">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="N3" s="10">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <f t="shared" ref="B4:B51" si="1">B3+A4</f>
+        <v>7</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" ref="C4:C51" si="2">C3+B4</f>
+        <v>14</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D51" si="3">D3+C4</f>
+        <v>25</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" ref="E4:E51" si="4">E3+D4</f>
+        <v>41</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" ref="F4:F51" si="5">F3+E4</f>
+        <v>63</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G51" si="6">G3+F4</f>
+        <v>92</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" ref="H4:H51" si="7">H3+G4</f>
+        <v>129</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" ref="I4:I51" si="8">I3+H4</f>
+        <v>175</v>
+      </c>
+      <c r="J4" s="10">
+        <f t="shared" ref="J4:J51" si="9">J3+I4</f>
+        <v>231</v>
+      </c>
+      <c r="K4" s="10">
+        <f t="shared" ref="K4:K51" si="10">K3+J4</f>
+        <v>298</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ref="L4:L51" si="11">L3+K4</f>
+        <v>377</v>
+      </c>
+      <c r="M4" s="10">
+        <f t="shared" ref="M4:M51" si="12">M3+L4</f>
+        <v>469</v>
+      </c>
+      <c r="N4" s="10">
+        <f t="shared" ref="N4:N51" si="13">N3+M4</f>
+        <v>575</v>
+      </c>
+      <c r="O4" s="10">
+        <f t="shared" ref="O4:O51" si="14">O3+N4</f>
+        <v>696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="5"/>
+        <v>154</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="6"/>
+        <v>246</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="7"/>
+        <v>375</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" si="8"/>
+        <v>550</v>
+      </c>
+      <c r="J5" s="10">
+        <f t="shared" si="9"/>
+        <v>781</v>
+      </c>
+      <c r="K5" s="10">
+        <f t="shared" si="10"/>
+        <v>1079</v>
+      </c>
+      <c r="L5" s="10">
+        <f t="shared" si="11"/>
+        <v>1456</v>
+      </c>
+      <c r="M5" s="10">
+        <f t="shared" si="12"/>
+        <v>1925</v>
+      </c>
+      <c r="N5" s="10">
+        <f t="shared" si="13"/>
+        <v>2500</v>
+      </c>
+      <c r="O5" s="10">
+        <f t="shared" si="14"/>
+        <v>3196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="10">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="4"/>
+        <v>182</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="5"/>
+        <v>336</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="6"/>
+        <v>582</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="7"/>
+        <v>957</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" si="8"/>
+        <v>1507</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="9"/>
+        <v>2288</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="10"/>
+        <v>3367</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" si="11"/>
+        <v>4823</v>
+      </c>
+      <c r="M6" s="10">
+        <f t="shared" si="12"/>
+        <v>6748</v>
+      </c>
+      <c r="N6" s="10">
+        <f t="shared" si="13"/>
+        <v>9248</v>
+      </c>
+      <c r="O6" s="10">
+        <f t="shared" si="14"/>
+        <v>12444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="4"/>
+        <v>336</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="5"/>
+        <v>672</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="6"/>
+        <v>1254</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="7"/>
+        <v>2211</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="8"/>
+        <v>3718</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="9"/>
+        <v>6006</v>
+      </c>
+      <c r="K7" s="10">
+        <f t="shared" si="10"/>
+        <v>9373</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" si="11"/>
+        <v>14196</v>
+      </c>
+      <c r="M7" s="10">
+        <f t="shared" si="12"/>
+        <v>20944</v>
+      </c>
+      <c r="N7" s="10">
+        <f t="shared" si="13"/>
+        <v>30192</v>
+      </c>
+      <c r="O7" s="10">
+        <f t="shared" si="14"/>
+        <v>42636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="3"/>
+        <v>246</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="4"/>
+        <v>582</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="5"/>
+        <v>1254</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="6"/>
+        <v>2508</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="7"/>
+        <v>4719</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="8"/>
+        <v>8437</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="9"/>
+        <v>14443</v>
+      </c>
+      <c r="K8" s="10">
+        <f t="shared" si="10"/>
+        <v>23816</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="11"/>
+        <v>38012</v>
+      </c>
+      <c r="M8" s="10">
+        <f t="shared" si="12"/>
+        <v>58956</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" si="13"/>
+        <v>89148</v>
+      </c>
+      <c r="O8" s="10">
+        <f t="shared" si="14"/>
+        <v>131784</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C9" s="10">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="3"/>
+        <v>375</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="4"/>
+        <v>957</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="5"/>
+        <v>2211</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" si="6"/>
+        <v>4719</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="7"/>
+        <v>9438</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="8"/>
+        <v>17875</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="9"/>
+        <v>32318</v>
+      </c>
+      <c r="K9" s="10">
+        <f t="shared" si="10"/>
+        <v>56134</v>
+      </c>
+      <c r="L9" s="10">
+        <f t="shared" si="11"/>
+        <v>94146</v>
+      </c>
+      <c r="M9" s="10">
+        <f t="shared" si="12"/>
+        <v>153102</v>
+      </c>
+      <c r="N9" s="10">
+        <f t="shared" si="13"/>
+        <v>242250</v>
+      </c>
+      <c r="O9" s="10">
+        <f t="shared" si="14"/>
+        <v>374034</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="C10" s="10">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="3"/>
+        <v>550</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="4"/>
+        <v>1507</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="5"/>
+        <v>3718</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="6"/>
+        <v>8437</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="7"/>
+        <v>17875</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="8"/>
+        <v>35750</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="9"/>
+        <v>68068</v>
+      </c>
+      <c r="K10" s="10">
+        <f t="shared" si="10"/>
+        <v>124202</v>
+      </c>
+      <c r="L10" s="10">
+        <f t="shared" si="11"/>
+        <v>218348</v>
+      </c>
+      <c r="M10" s="10">
+        <f t="shared" si="12"/>
+        <v>371450</v>
+      </c>
+      <c r="N10" s="10">
+        <f t="shared" si="13"/>
+        <v>613700</v>
+      </c>
+      <c r="O10" s="10">
+        <f t="shared" si="14"/>
+        <v>987734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="C11" s="10">
+        <f t="shared" si="2"/>
+        <v>231</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="3"/>
+        <v>781</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="4"/>
+        <v>2288</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="5"/>
+        <v>6006</v>
+      </c>
+      <c r="G11" s="10">
+        <f t="shared" si="6"/>
+        <v>14443</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="7"/>
+        <v>32318</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="8"/>
+        <v>68068</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="9"/>
+        <v>136136</v>
+      </c>
+      <c r="K11" s="10">
+        <f t="shared" si="10"/>
+        <v>260338</v>
+      </c>
+      <c r="L11" s="10">
+        <f t="shared" si="11"/>
+        <v>478686</v>
+      </c>
+      <c r="M11" s="10">
+        <f t="shared" si="12"/>
+        <v>850136</v>
+      </c>
+      <c r="N11" s="10">
+        <f t="shared" si="13"/>
+        <v>1463836</v>
+      </c>
+      <c r="O11" s="10">
+        <f t="shared" si="14"/>
+        <v>2451570</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="2"/>
+        <v>298</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="3"/>
+        <v>1079</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="4"/>
+        <v>3367</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="5"/>
+        <v>9373</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" si="6"/>
+        <v>23816</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="7"/>
+        <v>56134</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="8"/>
+        <v>124202</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="9"/>
+        <v>260338</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" si="10"/>
+        <v>520676</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="11"/>
+        <v>999362</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="12"/>
+        <v>1849498</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" si="13"/>
+        <v>3313334</v>
+      </c>
+      <c r="O12" s="10">
+        <f t="shared" si="14"/>
+        <v>5764904</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="C13" s="10">
+        <f t="shared" si="2"/>
+        <v>377</v>
+      </c>
+      <c r="D13" s="10">
+        <f t="shared" si="3"/>
+        <v>1456</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="4"/>
+        <v>4823</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="5"/>
+        <v>14196</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" si="6"/>
+        <v>38012</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="7"/>
+        <v>94146</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="8"/>
+        <v>218348</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" si="9"/>
+        <v>478686</v>
+      </c>
+      <c r="K13" s="10">
+        <f t="shared" si="10"/>
+        <v>999362</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="11"/>
+        <v>1998724</v>
+      </c>
+      <c r="M13" s="10">
+        <f t="shared" si="12"/>
+        <v>3848222</v>
+      </c>
+      <c r="N13" s="10">
+        <f t="shared" si="13"/>
+        <v>7161556</v>
+      </c>
+      <c r="O13" s="10">
+        <f t="shared" si="14"/>
+        <v>12926460</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="C14" s="10">
+        <f t="shared" si="2"/>
+        <v>469</v>
+      </c>
+      <c r="D14" s="10">
+        <f t="shared" si="3"/>
+        <v>1925</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="4"/>
+        <v>6748</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="5"/>
+        <v>20944</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="6"/>
+        <v>58956</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="7"/>
+        <v>153102</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="8"/>
+        <v>371450</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="9"/>
+        <v>850136</v>
+      </c>
+      <c r="K14" s="10">
+        <f t="shared" si="10"/>
+        <v>1849498</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="11"/>
+        <v>3848222</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="12"/>
+        <v>7696444</v>
+      </c>
+      <c r="N14" s="10">
+        <f t="shared" si="13"/>
+        <v>14858000</v>
+      </c>
+      <c r="O14" s="10">
+        <f t="shared" si="14"/>
+        <v>27784460</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="C15" s="10">
+        <f t="shared" si="2"/>
+        <v>575</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" si="3"/>
+        <v>2500</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="4"/>
+        <v>9248</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="5"/>
+        <v>30192</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="6"/>
+        <v>89148</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="7"/>
+        <v>242250</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="8"/>
+        <v>613700</v>
+      </c>
+      <c r="J15" s="10">
+        <f t="shared" si="9"/>
+        <v>1463836</v>
+      </c>
+      <c r="K15" s="10">
+        <f t="shared" si="10"/>
+        <v>3313334</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="11"/>
+        <v>7161556</v>
+      </c>
+      <c r="M15" s="10">
+        <f t="shared" si="12"/>
+        <v>14858000</v>
+      </c>
+      <c r="N15" s="10">
+        <f t="shared" si="13"/>
+        <v>29716000</v>
+      </c>
+      <c r="O15" s="10">
+        <f t="shared" si="14"/>
+        <v>57500460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="C16" s="10">
+        <f t="shared" si="2"/>
+        <v>696</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="3"/>
+        <v>3196</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="4"/>
+        <v>12444</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="5"/>
+        <v>42636</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="6"/>
+        <v>131784</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="7"/>
+        <v>374034</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="8"/>
+        <v>987734</v>
+      </c>
+      <c r="J16" s="10">
+        <f t="shared" si="9"/>
+        <v>2451570</v>
+      </c>
+      <c r="K16" s="10">
+        <f t="shared" si="10"/>
+        <v>5764904</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="11"/>
+        <v>12926460</v>
+      </c>
+      <c r="M16" s="10">
+        <f t="shared" si="12"/>
+        <v>27784460</v>
+      </c>
+      <c r="N16" s="10">
+        <f t="shared" si="13"/>
+        <v>57500460</v>
+      </c>
+      <c r="O16" s="10">
+        <f t="shared" si="14"/>
+        <v>115000920</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="C17" s="10">
+        <f t="shared" si="2"/>
+        <v>833</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" si="3"/>
+        <v>4029</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="4"/>
+        <v>16473</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="5"/>
+        <v>59109</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="6"/>
+        <v>190893</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="7"/>
+        <v>564927</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="8"/>
+        <v>1552661</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" si="9"/>
+        <v>4004231</v>
+      </c>
+      <c r="K17" s="10">
+        <f t="shared" si="10"/>
+        <v>9769135</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="11"/>
+        <v>22695595</v>
+      </c>
+      <c r="M17" s="10">
+        <f t="shared" si="12"/>
+        <v>50480055</v>
+      </c>
+      <c r="N17" s="10">
+        <f t="shared" si="13"/>
+        <v>107980515</v>
+      </c>
+      <c r="O17" s="10">
+        <f t="shared" si="14"/>
+        <v>222981435</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+      <c r="C18" s="10">
+        <f t="shared" si="2"/>
+        <v>987</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="3"/>
+        <v>5016</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="4"/>
+        <v>21489</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="5"/>
+        <v>80598</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="6"/>
+        <v>271491</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="7"/>
+        <v>836418</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="8"/>
+        <v>2389079</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="9"/>
+        <v>6393310</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10">
+        <f t="shared" si="1"/>
+        <v>172</v>
+      </c>
+      <c r="C19" s="10">
+        <f t="shared" si="2"/>
+        <v>1159</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" si="3"/>
+        <v>6175</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="4"/>
+        <v>27664</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="5"/>
+        <v>108262</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" si="6"/>
+        <v>379753</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="7"/>
+        <v>1216171</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="8"/>
+        <v>3605250</v>
+      </c>
+      <c r="O19" s="10">
+        <f t="shared" ref="O19:O26" si="15">O20+O21</f>
+        <v>5702887</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="C20" s="10">
+        <f t="shared" si="2"/>
+        <v>1350</v>
+      </c>
+      <c r="D20" s="10">
+        <f t="shared" si="3"/>
+        <v>7525</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="4"/>
+        <v>35189</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="5"/>
+        <v>143451</v>
+      </c>
+      <c r="G20" s="10">
+        <f t="shared" si="6"/>
+        <v>523204</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="7"/>
+        <v>1739375</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="8"/>
+        <v>5344625</v>
+      </c>
+      <c r="J20" s="13">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="K20" s="10">
+        <f t="shared" ref="K19:K26" si="16">L20+K21</f>
+        <v>78175076</v>
+      </c>
+      <c r="L20" s="10">
+        <f t="shared" ref="L19:L26" si="17">M20+L21</f>
+        <v>29860634</v>
+      </c>
+      <c r="M20" s="10">
+        <f t="shared" ref="M19:M26" si="18">N20+M21</f>
+        <v>11405772</v>
+      </c>
+      <c r="N20" s="10">
+        <f t="shared" ref="N19:N26" si="19">N21+N22</f>
+        <v>4356618</v>
+      </c>
+      <c r="O20" s="10">
+        <f t="shared" si="15"/>
+        <v>3524578</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10">
+        <f t="shared" si="1"/>
+        <v>211</v>
+      </c>
+      <c r="C21" s="10">
+        <f t="shared" si="2"/>
+        <v>1561</v>
+      </c>
+      <c r="D21" s="10">
+        <f t="shared" si="3"/>
+        <v>9086</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="4"/>
+        <v>44275</v>
+      </c>
+      <c r="F21" s="10">
+        <f t="shared" si="5"/>
+        <v>187726</v>
+      </c>
+      <c r="G21" s="10">
+        <f t="shared" si="6"/>
+        <v>710930</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="7"/>
+        <v>2450305</v>
+      </c>
+      <c r="I21" s="10">
+        <f t="shared" si="8"/>
+        <v>7794930</v>
+      </c>
+      <c r="J21" s="12">
+        <v>26640</v>
+      </c>
+      <c r="K21" s="10">
+        <f t="shared" si="16"/>
+        <v>48314442</v>
+      </c>
+      <c r="L21" s="10">
+        <f t="shared" si="17"/>
+        <v>18454862</v>
+      </c>
+      <c r="M21" s="10">
+        <f t="shared" si="18"/>
+        <v>7049154</v>
+      </c>
+      <c r="N21" s="10">
+        <f t="shared" si="19"/>
+        <v>2692538</v>
+      </c>
+      <c r="O21" s="10">
+        <f t="shared" si="15"/>
+        <v>2178309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10">
+        <f t="shared" si="1"/>
+        <v>232</v>
+      </c>
+      <c r="C22" s="10">
+        <f t="shared" si="2"/>
+        <v>1793</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" si="3"/>
+        <v>10879</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="4"/>
+        <v>55154</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" si="5"/>
+        <v>242880</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="6"/>
+        <v>953810</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="7"/>
+        <v>3404115</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="8"/>
+        <v>11199045</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" ref="J19:J26" si="20">K22+J23</f>
+        <v>78163168</v>
+      </c>
+      <c r="K22" s="10">
+        <f t="shared" si="16"/>
+        <v>29859580</v>
+      </c>
+      <c r="L22" s="10">
+        <f t="shared" si="17"/>
+        <v>11405708</v>
+      </c>
+      <c r="M22" s="10">
+        <f t="shared" si="18"/>
+        <v>4356616</v>
+      </c>
+      <c r="N22" s="10">
+        <f t="shared" si="19"/>
+        <v>1664080</v>
+      </c>
+      <c r="O22" s="10">
+        <f t="shared" si="15"/>
+        <v>1346269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10">
+        <f t="shared" si="1"/>
+        <v>254</v>
+      </c>
+      <c r="C23" s="10">
+        <f t="shared" si="2"/>
+        <v>2047</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="3"/>
+        <v>12926</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="4"/>
+        <v>68080</v>
+      </c>
+      <c r="F23" s="10">
+        <f t="shared" si="5"/>
+        <v>310960</v>
+      </c>
+      <c r="G23" s="10">
+        <f t="shared" si="6"/>
+        <v>1264770</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" si="7"/>
+        <v>4668885</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="8"/>
+        <v>15867930</v>
+      </c>
+      <c r="J23" s="10">
+        <f t="shared" si="20"/>
+        <v>48303588</v>
+      </c>
+      <c r="K23" s="10">
+        <f t="shared" si="16"/>
+        <v>18453872</v>
+      </c>
+      <c r="L23" s="10">
+        <f t="shared" si="17"/>
+        <v>7049092</v>
+      </c>
+      <c r="M23" s="10">
+        <f t="shared" si="18"/>
+        <v>2692536</v>
+      </c>
+      <c r="N23" s="10">
+        <f t="shared" si="19"/>
+        <v>1028458</v>
+      </c>
+      <c r="O23" s="10">
+        <f t="shared" si="15"/>
+        <v>832040</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" si="2"/>
+        <v>2324</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="3"/>
+        <v>15250</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="4"/>
+        <v>83330</v>
+      </c>
+      <c r="F24" s="10">
+        <f t="shared" si="5"/>
+        <v>394290</v>
+      </c>
+      <c r="G24" s="10">
+        <f t="shared" si="6"/>
+        <v>1659060</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="7"/>
+        <v>6327945</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="8"/>
+        <v>22195875</v>
+      </c>
+      <c r="J24" s="10">
+        <f t="shared" si="20"/>
+        <v>29849716</v>
+      </c>
+      <c r="K24" s="10">
+        <f t="shared" si="16"/>
+        <v>11404780</v>
+      </c>
+      <c r="L24" s="10">
+        <f t="shared" si="17"/>
+        <v>4356556</v>
+      </c>
+      <c r="M24" s="10">
+        <f t="shared" si="18"/>
+        <v>1664078</v>
+      </c>
+      <c r="N24" s="10">
+        <f t="shared" si="19"/>
+        <v>635622</v>
+      </c>
+      <c r="O24" s="10">
+        <f t="shared" si="15"/>
+        <v>514229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10">
+        <f t="shared" si="1"/>
+        <v>301</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
+      <c r="D25" s="10">
+        <f t="shared" si="3"/>
+        <v>17875</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="4"/>
+        <v>101205</v>
+      </c>
+      <c r="F25" s="10">
+        <f t="shared" si="5"/>
+        <v>495495</v>
+      </c>
+      <c r="G25" s="10">
+        <f t="shared" si="6"/>
+        <v>2154555</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="7"/>
+        <v>8482500</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="8"/>
+        <v>30678375</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="20"/>
+        <v>18444936</v>
+      </c>
+      <c r="K25" s="10">
+        <f t="shared" si="16"/>
+        <v>7048224</v>
+      </c>
+      <c r="L25" s="10">
+        <f t="shared" si="17"/>
+        <v>2692478</v>
+      </c>
+      <c r="M25" s="10">
+        <f t="shared" si="18"/>
+        <v>1028456</v>
+      </c>
+      <c r="N25" s="10">
+        <f t="shared" si="19"/>
+        <v>392836</v>
+      </c>
+      <c r="O25" s="10">
+        <f t="shared" si="15"/>
+        <v>317811</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10">
+        <f t="shared" si="1"/>
+        <v>326</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="2"/>
+        <v>2951</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" si="3"/>
+        <v>20826</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="4"/>
+        <v>122031</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="5"/>
+        <v>617526</v>
+      </c>
+      <c r="G26" s="10">
+        <f t="shared" si="6"/>
+        <v>2772081</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="7"/>
+        <v>11254581</v>
+      </c>
+      <c r="I26" s="10">
+        <f t="shared" si="8"/>
+        <v>41932956</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" si="20"/>
+        <v>11396712</v>
+      </c>
+      <c r="K26" s="10">
+        <f t="shared" si="16"/>
+        <v>4355746</v>
+      </c>
+      <c r="L26" s="10">
+        <f t="shared" si="17"/>
+        <v>1664022</v>
+      </c>
+      <c r="M26" s="10">
+        <f t="shared" si="18"/>
+        <v>635620</v>
+      </c>
+      <c r="N26" s="10">
+        <f t="shared" si="19"/>
+        <v>242786</v>
+      </c>
+      <c r="O26" s="10">
+        <f t="shared" si="15"/>
+        <v>196418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10">
+        <f t="shared" si="1"/>
+        <v>352</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="2"/>
+        <v>3303</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" si="3"/>
+        <v>24129</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="4"/>
+        <v>146160</v>
+      </c>
+      <c r="F27" s="10">
+        <f t="shared" si="5"/>
+        <v>763686</v>
+      </c>
+      <c r="G27" s="10">
+        <f t="shared" si="6"/>
+        <v>3535767</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="7"/>
+        <v>14790348</v>
+      </c>
+      <c r="I27" s="10">
+        <f t="shared" ref="G27:I48" si="21">J27+I28</f>
+        <v>18390774</v>
+      </c>
+      <c r="J27" s="10">
+        <f t="shared" ref="J27:J48" si="22">K27+J28</f>
+        <v>7040966</v>
+      </c>
+      <c r="K27" s="10">
+        <f t="shared" ref="K27:K48" si="23">L27+K28</f>
+        <v>2691724</v>
+      </c>
+      <c r="L27" s="10">
+        <f t="shared" ref="L27:L48" si="24">M27+L28</f>
+        <v>1028402</v>
+      </c>
+      <c r="M27" s="10">
+        <f t="shared" ref="M27:M48" si="25">N27+M28</f>
+        <v>392834</v>
+      </c>
+      <c r="N27" s="10">
+        <f t="shared" ref="N27:N48" si="26">N28+N29</f>
+        <v>150050</v>
+      </c>
+      <c r="O27" s="10">
+        <f t="shared" ref="O27:O48" si="27">O28+O29</f>
+        <v>121393</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10">
+        <f t="shared" si="1"/>
+        <v>379</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="2"/>
+        <v>3682</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" si="3"/>
+        <v>27811</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="4"/>
+        <v>173971</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" si="5"/>
+        <v>937657</v>
+      </c>
+      <c r="G28" s="10">
+        <f t="shared" si="6"/>
+        <v>4473424</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="7"/>
+        <v>19263772</v>
+      </c>
+      <c r="I28" s="10">
+        <f t="shared" si="21"/>
+        <v>11349808</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="22"/>
+        <v>4349242</v>
+      </c>
+      <c r="K28" s="10">
+        <f t="shared" si="23"/>
+        <v>1663322</v>
+      </c>
+      <c r="L28" s="10">
+        <f t="shared" si="24"/>
+        <v>635568</v>
+      </c>
+      <c r="M28" s="10">
+        <f t="shared" si="25"/>
+        <v>242784</v>
+      </c>
+      <c r="N28" s="10">
+        <f t="shared" si="26"/>
+        <v>92736</v>
+      </c>
+      <c r="O28" s="10">
+        <f t="shared" si="27"/>
+        <v>75025</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10">
+        <f t="shared" si="1"/>
+        <v>407</v>
+      </c>
+      <c r="C29" s="10">
+        <f t="shared" si="2"/>
+        <v>4089</v>
+      </c>
+      <c r="D29" s="10">
+        <f t="shared" si="3"/>
+        <v>31900</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" si="4"/>
+        <v>205871</v>
+      </c>
+      <c r="F29" s="10">
+        <f t="shared" si="5"/>
+        <v>1143528</v>
+      </c>
+      <c r="G29" s="10">
+        <f t="shared" si="6"/>
+        <v>5616952</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="7"/>
+        <v>24880724</v>
+      </c>
+      <c r="I29" s="10">
+        <f t="shared" si="21"/>
+        <v>7000566</v>
+      </c>
+      <c r="J29" s="10">
+        <f t="shared" si="22"/>
+        <v>2685920</v>
+      </c>
+      <c r="K29" s="10">
+        <f t="shared" si="23"/>
+        <v>1027754</v>
+      </c>
+      <c r="L29" s="10">
+        <f t="shared" si="24"/>
+        <v>392784</v>
+      </c>
+      <c r="M29" s="10">
+        <f t="shared" si="25"/>
+        <v>150048</v>
+      </c>
+      <c r="N29" s="10">
+        <f t="shared" si="26"/>
+        <v>57314</v>
+      </c>
+      <c r="O29" s="10">
+        <f t="shared" si="27"/>
+        <v>46368</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="10">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10">
+        <f t="shared" si="1"/>
+        <v>436</v>
+      </c>
+      <c r="C30" s="10">
+        <f t="shared" si="2"/>
+        <v>4525</v>
+      </c>
+      <c r="D30" s="10">
+        <f t="shared" si="3"/>
+        <v>36425</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="4"/>
+        <v>242296</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="5"/>
+        <v>1385824</v>
+      </c>
+      <c r="G30" s="10">
+        <f t="shared" si="6"/>
+        <v>7002776</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="7"/>
+        <v>31883500</v>
+      </c>
+      <c r="I30" s="10">
+        <f t="shared" si="21"/>
+        <v>4314646</v>
+      </c>
+      <c r="J30" s="10">
+        <f t="shared" si="22"/>
+        <v>1658166</v>
+      </c>
+      <c r="K30" s="10">
+        <f t="shared" si="23"/>
+        <v>634970</v>
+      </c>
+      <c r="L30" s="10">
+        <f t="shared" si="24"/>
+        <v>242736</v>
+      </c>
+      <c r="M30" s="10">
+        <f t="shared" si="25"/>
+        <v>92734</v>
+      </c>
+      <c r="N30" s="10">
+        <f t="shared" si="26"/>
+        <v>35422</v>
+      </c>
+      <c r="O30" s="10">
+        <f t="shared" si="27"/>
+        <v>28657</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="10">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10">
+        <f t="shared" si="1"/>
+        <v>466</v>
+      </c>
+      <c r="C31" s="10">
+        <f t="shared" si="2"/>
+        <v>4991</v>
+      </c>
+      <c r="D31" s="10">
+        <f t="shared" si="3"/>
+        <v>41416</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="4"/>
+        <v>283712</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" si="5"/>
+        <v>1669536</v>
+      </c>
+      <c r="G31" s="10">
+        <f t="shared" si="6"/>
+        <v>8672312</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="7"/>
+        <v>40555812</v>
+      </c>
+      <c r="I31" s="10">
+        <f t="shared" si="21"/>
+        <v>2656480</v>
+      </c>
+      <c r="J31" s="10">
+        <f t="shared" si="22"/>
+        <v>1023196</v>
+      </c>
+      <c r="K31" s="10">
+        <f t="shared" si="23"/>
+        <v>392234</v>
+      </c>
+      <c r="L31" s="10">
+        <f t="shared" si="24"/>
+        <v>150002</v>
+      </c>
+      <c r="M31" s="10">
+        <f t="shared" si="25"/>
+        <v>57312</v>
+      </c>
+      <c r="N31" s="10">
+        <f t="shared" si="26"/>
+        <v>21892</v>
+      </c>
+      <c r="O31" s="10">
+        <f t="shared" si="27"/>
+        <v>17711</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10">
+        <f t="shared" si="1"/>
+        <v>497</v>
+      </c>
+      <c r="C32" s="10">
+        <f t="shared" si="2"/>
+        <v>5488</v>
+      </c>
+      <c r="D32" s="10">
+        <f t="shared" si="3"/>
+        <v>46904</v>
+      </c>
+      <c r="E32" s="10">
+        <f t="shared" si="4"/>
+        <v>330616</v>
+      </c>
+      <c r="F32" s="10">
+        <f t="shared" si="5"/>
+        <v>2000152</v>
+      </c>
+      <c r="G32" s="10">
+        <f t="shared" si="6"/>
+        <v>10672464</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" si="7"/>
+        <v>51228276</v>
+      </c>
+      <c r="I32" s="10">
+        <f t="shared" si="21"/>
+        <v>1633284</v>
+      </c>
+      <c r="J32" s="10">
+        <f t="shared" si="22"/>
+        <v>630962</v>
+      </c>
+      <c r="K32" s="10">
+        <f t="shared" si="23"/>
+        <v>242232</v>
+      </c>
+      <c r="L32" s="10">
+        <f t="shared" si="24"/>
+        <v>92690</v>
+      </c>
+      <c r="M32" s="10">
+        <f t="shared" si="25"/>
+        <v>35420</v>
+      </c>
+      <c r="N32" s="10">
+        <f t="shared" si="26"/>
+        <v>13530</v>
+      </c>
+      <c r="O32" s="10">
+        <f t="shared" si="27"/>
+        <v>10946</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="10">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10">
+        <f t="shared" si="1"/>
+        <v>529</v>
+      </c>
+      <c r="C33" s="10">
+        <f t="shared" si="2"/>
+        <v>6017</v>
+      </c>
+      <c r="D33" s="10">
+        <f t="shared" ref="D33:D49" si="28">E33+D34</f>
+        <v>88528682</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" ref="E33:E49" si="29">F33+E34</f>
+        <v>37742426</v>
+      </c>
+      <c r="F33" s="10">
+        <f t="shared" ref="F33:F49" si="30">G33+F34</f>
+        <v>15711614</v>
+      </c>
+      <c r="G33" s="10">
+        <f t="shared" si="21"/>
+        <v>6396218</v>
+      </c>
+      <c r="H33" s="10">
+        <f t="shared" si="21"/>
+        <v>2552834</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="21"/>
+        <v>1002322</v>
+      </c>
+      <c r="J33" s="10">
+        <f t="shared" si="22"/>
+        <v>388730</v>
+      </c>
+      <c r="K33" s="10">
+        <f t="shared" si="23"/>
+        <v>149542</v>
+      </c>
+      <c r="L33" s="10">
+        <f t="shared" si="24"/>
+        <v>57270</v>
+      </c>
+      <c r="M33" s="10">
+        <f t="shared" si="25"/>
+        <v>21890</v>
+      </c>
+      <c r="N33" s="10">
+        <f t="shared" si="26"/>
+        <v>8362</v>
+      </c>
+      <c r="O33" s="10">
+        <f t="shared" si="27"/>
+        <v>6765</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="10">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10">
+        <f t="shared" si="1"/>
+        <v>562</v>
+      </c>
+      <c r="C34" s="10">
+        <f t="shared" si="2"/>
+        <v>6579</v>
+      </c>
+      <c r="D34" s="10">
+        <f t="shared" si="28"/>
+        <v>50786256</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="29"/>
+        <v>22030812</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="30"/>
+        <v>9315396</v>
+      </c>
+      <c r="G34" s="10">
+        <f t="shared" si="21"/>
+        <v>3843384</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="21"/>
+        <v>1550512</v>
+      </c>
+      <c r="I34" s="10">
+        <f t="shared" si="21"/>
+        <v>613592</v>
+      </c>
+      <c r="J34" s="10">
+        <f t="shared" si="22"/>
+        <v>239188</v>
+      </c>
+      <c r="K34" s="10">
+        <f t="shared" si="23"/>
+        <v>92272</v>
+      </c>
+      <c r="L34" s="10">
+        <f t="shared" si="24"/>
+        <v>35380</v>
+      </c>
+      <c r="M34" s="10">
+        <f t="shared" si="25"/>
+        <v>13528</v>
+      </c>
+      <c r="N34" s="10">
+        <f t="shared" si="26"/>
+        <v>5168</v>
+      </c>
+      <c r="O34" s="10">
+        <f t="shared" si="27"/>
+        <v>4181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="10">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10">
+        <f t="shared" si="1"/>
+        <v>596</v>
+      </c>
+      <c r="C35" s="10">
+        <f t="shared" si="2"/>
+        <v>7175</v>
+      </c>
+      <c r="D35" s="10">
+        <f t="shared" si="28"/>
+        <v>28755444</v>
+      </c>
+      <c r="E35" s="10">
+        <f t="shared" si="29"/>
+        <v>12715416</v>
+      </c>
+      <c r="F35" s="10">
+        <f t="shared" si="30"/>
+        <v>5472012</v>
+      </c>
+      <c r="G35" s="10">
+        <f t="shared" si="21"/>
+        <v>2292872</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="21"/>
+        <v>936920</v>
+      </c>
+      <c r="I35" s="10">
+        <f t="shared" si="21"/>
+        <v>374404</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" si="22"/>
+        <v>146916</v>
+      </c>
+      <c r="K35" s="10">
+        <f t="shared" si="23"/>
+        <v>56892</v>
+      </c>
+      <c r="L35" s="10">
+        <f t="shared" si="24"/>
+        <v>21852</v>
+      </c>
+      <c r="M35" s="10">
+        <f t="shared" si="25"/>
+        <v>8360</v>
+      </c>
+      <c r="N35" s="10">
+        <f t="shared" si="26"/>
+        <v>3194</v>
+      </c>
+      <c r="O35" s="10">
+        <f t="shared" si="27"/>
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="10">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10">
+        <f t="shared" si="1"/>
+        <v>631</v>
+      </c>
+      <c r="C36" s="10">
+        <f t="shared" si="2"/>
+        <v>7806</v>
+      </c>
+      <c r="D36" s="10">
+        <f t="shared" si="28"/>
+        <v>16040028</v>
+      </c>
+      <c r="E36" s="10">
+        <f t="shared" si="29"/>
+        <v>7243404</v>
+      </c>
+      <c r="F36" s="10">
+        <f t="shared" si="30"/>
+        <v>3179140</v>
+      </c>
+      <c r="G36" s="10">
+        <f t="shared" si="21"/>
+        <v>1355952</v>
+      </c>
+      <c r="H36" s="10">
+        <f t="shared" si="21"/>
+        <v>562516</v>
+      </c>
+      <c r="I36" s="10">
+        <f t="shared" si="21"/>
+        <v>227488</v>
+      </c>
+      <c r="J36" s="10">
+        <f t="shared" si="22"/>
+        <v>90024</v>
+      </c>
+      <c r="K36" s="10">
+        <f t="shared" si="23"/>
+        <v>35040</v>
+      </c>
+      <c r="L36" s="10">
+        <f t="shared" si="24"/>
+        <v>13492</v>
+      </c>
+      <c r="M36" s="10">
+        <f t="shared" si="25"/>
+        <v>5166</v>
+      </c>
+      <c r="N36" s="10">
+        <f t="shared" si="26"/>
+        <v>1974</v>
+      </c>
+      <c r="O36" s="10">
+        <f t="shared" si="27"/>
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="10">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10">
+        <f t="shared" si="1"/>
+        <v>667</v>
+      </c>
+      <c r="C37" s="10">
+        <f t="shared" si="2"/>
+        <v>8473</v>
+      </c>
+      <c r="D37" s="10">
+        <f t="shared" si="28"/>
+        <v>8796624</v>
+      </c>
+      <c r="E37" s="10">
+        <f t="shared" si="29"/>
+        <v>4064264</v>
+      </c>
+      <c r="F37" s="10">
+        <f t="shared" si="30"/>
+        <v>1823188</v>
+      </c>
+      <c r="G37" s="10">
+        <f t="shared" si="21"/>
+        <v>793436</v>
+      </c>
+      <c r="H37" s="10">
+        <f t="shared" si="21"/>
+        <v>335028</v>
+      </c>
+      <c r="I37" s="10">
+        <f t="shared" si="21"/>
+        <v>137464</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="22"/>
+        <v>54984</v>
+      </c>
+      <c r="K37" s="10">
+        <f t="shared" si="23"/>
+        <v>21548</v>
+      </c>
+      <c r="L37" s="10">
+        <f t="shared" si="24"/>
+        <v>8326</v>
+      </c>
+      <c r="M37" s="10">
+        <f t="shared" si="25"/>
+        <v>3192</v>
+      </c>
+      <c r="N37" s="10">
+        <f t="shared" si="26"/>
+        <v>1220</v>
+      </c>
+      <c r="O37" s="10">
+        <f t="shared" si="27"/>
+        <v>987</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="10">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10">
+        <f t="shared" si="1"/>
+        <v>704</v>
+      </c>
+      <c r="C38" s="10">
+        <f t="shared" si="2"/>
+        <v>9177</v>
+      </c>
+      <c r="D38" s="10">
+        <f t="shared" si="28"/>
+        <v>4732360</v>
+      </c>
+      <c r="E38" s="10">
+        <f t="shared" si="29"/>
+        <v>2241076</v>
+      </c>
+      <c r="F38" s="10">
+        <f t="shared" si="30"/>
+        <v>1029752</v>
+      </c>
+      <c r="G38" s="10">
+        <f t="shared" si="21"/>
+        <v>458408</v>
+      </c>
+      <c r="H38" s="10">
+        <f t="shared" si="21"/>
+        <v>197564</v>
+      </c>
+      <c r="I38" s="10">
+        <f t="shared" si="21"/>
+        <v>82480</v>
+      </c>
+      <c r="J38" s="10">
+        <f t="shared" si="22"/>
+        <v>33436</v>
+      </c>
+      <c r="K38" s="10">
+        <f t="shared" si="23"/>
+        <v>13222</v>
+      </c>
+      <c r="L38" s="10">
+        <f t="shared" si="24"/>
+        <v>5134</v>
+      </c>
+      <c r="M38" s="10">
+        <f t="shared" si="25"/>
+        <v>1972</v>
+      </c>
+      <c r="N38" s="10">
+        <f t="shared" si="26"/>
+        <v>754</v>
+      </c>
+      <c r="O38" s="10">
+        <f t="shared" si="27"/>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="10">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10">
+        <f t="shared" si="1"/>
+        <v>742</v>
+      </c>
+      <c r="C39" s="10">
+        <f t="shared" si="2"/>
+        <v>9919</v>
+      </c>
+      <c r="D39" s="10">
+        <f t="shared" si="28"/>
+        <v>2491284</v>
+      </c>
+      <c r="E39" s="10">
+        <f t="shared" si="29"/>
+        <v>1211324</v>
+      </c>
+      <c r="F39" s="10">
+        <f t="shared" si="30"/>
+        <v>571344</v>
+      </c>
+      <c r="G39" s="10">
+        <f t="shared" si="21"/>
+        <v>260844</v>
+      </c>
+      <c r="H39" s="10">
+        <f t="shared" si="21"/>
+        <v>115084</v>
+      </c>
+      <c r="I39" s="10">
+        <f t="shared" si="21"/>
+        <v>49044</v>
+      </c>
+      <c r="J39" s="10">
+        <f t="shared" si="22"/>
+        <v>20214</v>
+      </c>
+      <c r="K39" s="10">
+        <f t="shared" si="23"/>
+        <v>8088</v>
+      </c>
+      <c r="L39" s="10">
+        <f t="shared" si="24"/>
+        <v>3162</v>
+      </c>
+      <c r="M39" s="10">
+        <f t="shared" si="25"/>
+        <v>1218</v>
+      </c>
+      <c r="N39" s="10">
+        <f t="shared" si="26"/>
+        <v>466</v>
+      </c>
+      <c r="O39" s="10">
+        <f t="shared" si="27"/>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="10">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10">
+        <f t="shared" si="1"/>
+        <v>781</v>
+      </c>
+      <c r="C40" s="10">
+        <f t="shared" si="2"/>
+        <v>10700</v>
+      </c>
+      <c r="D40" s="10">
+        <f t="shared" si="28"/>
+        <v>1279960</v>
+      </c>
+      <c r="E40" s="10">
+        <f t="shared" si="29"/>
+        <v>639980</v>
+      </c>
+      <c r="F40" s="10">
+        <f t="shared" si="30"/>
+        <v>310500</v>
+      </c>
+      <c r="G40" s="10">
+        <f t="shared" si="21"/>
+        <v>145760</v>
+      </c>
+      <c r="H40" s="10">
+        <f t="shared" si="21"/>
+        <v>66040</v>
+      </c>
+      <c r="I40" s="10">
+        <f t="shared" si="21"/>
+        <v>28830</v>
+      </c>
+      <c r="J40" s="10">
+        <f t="shared" si="22"/>
+        <v>12126</v>
+      </c>
+      <c r="K40" s="10">
+        <f t="shared" si="23"/>
+        <v>4926</v>
+      </c>
+      <c r="L40" s="10">
+        <f t="shared" si="24"/>
+        <v>1944</v>
+      </c>
+      <c r="M40" s="10">
+        <f t="shared" si="25"/>
+        <v>752</v>
+      </c>
+      <c r="N40" s="10">
+        <f t="shared" si="26"/>
+        <v>288</v>
+      </c>
+      <c r="O40" s="10">
+        <f t="shared" si="27"/>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="10">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10">
+        <f t="shared" si="1"/>
+        <v>821</v>
+      </c>
+      <c r="C41" s="10">
+        <f t="shared" si="2"/>
+        <v>11521</v>
+      </c>
+      <c r="D41" s="10">
+        <f t="shared" si="28"/>
+        <v>639980</v>
+      </c>
+      <c r="E41" s="10">
+        <f t="shared" si="29"/>
+        <v>329480</v>
+      </c>
+      <c r="F41" s="10">
+        <f t="shared" si="30"/>
+        <v>164740</v>
+      </c>
+      <c r="G41" s="10">
+        <f t="shared" si="21"/>
+        <v>79720</v>
+      </c>
+      <c r="H41" s="10">
+        <f t="shared" si="21"/>
+        <v>37210</v>
+      </c>
+      <c r="I41" s="10">
+        <f t="shared" si="21"/>
+        <v>16704</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="22"/>
+        <v>7200</v>
+      </c>
+      <c r="K41" s="10">
+        <f t="shared" si="23"/>
+        <v>2982</v>
+      </c>
+      <c r="L41" s="10">
+        <f t="shared" si="24"/>
+        <v>1192</v>
+      </c>
+      <c r="M41" s="10">
+        <f t="shared" si="25"/>
+        <v>464</v>
+      </c>
+      <c r="N41" s="10">
+        <f t="shared" si="26"/>
+        <v>178</v>
+      </c>
+      <c r="O41" s="10">
+        <f t="shared" si="27"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="10">
+        <v>41</v>
+      </c>
+      <c r="B42" s="10">
+        <f t="shared" si="1"/>
+        <v>862</v>
+      </c>
+      <c r="C42" s="10">
+        <f t="shared" si="2"/>
+        <v>12383</v>
+      </c>
+      <c r="D42" s="10">
+        <f t="shared" si="28"/>
+        <v>310500</v>
+      </c>
+      <c r="E42" s="10">
+        <f t="shared" si="29"/>
+        <v>164740</v>
+      </c>
+      <c r="F42" s="10">
+        <f t="shared" si="30"/>
+        <v>85020</v>
+      </c>
+      <c r="G42" s="10">
+        <f t="shared" si="21"/>
+        <v>42510</v>
+      </c>
+      <c r="H42" s="10">
+        <f t="shared" si="21"/>
+        <v>20506</v>
+      </c>
+      <c r="I42" s="10">
+        <f t="shared" si="21"/>
+        <v>9504</v>
+      </c>
+      <c r="J42" s="10">
+        <f t="shared" si="22"/>
+        <v>4218</v>
+      </c>
+      <c r="K42" s="10">
+        <f t="shared" si="23"/>
+        <v>1790</v>
+      </c>
+      <c r="L42" s="10">
+        <f t="shared" si="24"/>
+        <v>728</v>
+      </c>
+      <c r="M42" s="10">
+        <f t="shared" si="25"/>
+        <v>286</v>
+      </c>
+      <c r="N42" s="10">
+        <f t="shared" si="26"/>
+        <v>110</v>
+      </c>
+      <c r="O42" s="10">
+        <f t="shared" si="27"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="10">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10">
+        <f t="shared" si="1"/>
+        <v>904</v>
+      </c>
+      <c r="C43" s="10">
+        <f t="shared" si="2"/>
+        <v>13287</v>
+      </c>
+      <c r="D43" s="10">
+        <f t="shared" si="28"/>
+        <v>145760</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="29"/>
+        <v>79720</v>
+      </c>
+      <c r="F43" s="10">
+        <f t="shared" si="30"/>
+        <v>42510</v>
+      </c>
+      <c r="G43" s="10">
+        <f t="shared" si="21"/>
+        <v>22004</v>
+      </c>
+      <c r="H43" s="10">
+        <f t="shared" si="21"/>
+        <v>11002</v>
+      </c>
+      <c r="I43" s="10">
+        <f t="shared" si="21"/>
+        <v>5286</v>
+      </c>
+      <c r="J43" s="10">
+        <f t="shared" si="22"/>
+        <v>2428</v>
+      </c>
+      <c r="K43" s="10">
+        <f t="shared" si="23"/>
+        <v>1062</v>
+      </c>
+      <c r="L43" s="10">
+        <f t="shared" si="24"/>
+        <v>442</v>
+      </c>
+      <c r="M43" s="10">
+        <f t="shared" si="25"/>
+        <v>176</v>
+      </c>
+      <c r="N43" s="10">
+        <f t="shared" si="26"/>
+        <v>68</v>
+      </c>
+      <c r="O43" s="10">
+        <f t="shared" si="27"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="10">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10">
+        <f t="shared" si="1"/>
+        <v>947</v>
+      </c>
+      <c r="C44" s="10">
+        <f t="shared" si="2"/>
+        <v>14234</v>
+      </c>
+      <c r="D44" s="10">
+        <f t="shared" si="28"/>
+        <v>66040</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="29"/>
+        <v>37210</v>
+      </c>
+      <c r="F44" s="10">
+        <f t="shared" si="30"/>
+        <v>20506</v>
+      </c>
+      <c r="G44" s="10">
+        <f t="shared" si="21"/>
+        <v>11002</v>
+      </c>
+      <c r="H44" s="10">
+        <f t="shared" si="21"/>
+        <v>5716</v>
+      </c>
+      <c r="I44" s="10">
+        <f t="shared" si="21"/>
+        <v>2858</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="22"/>
+        <v>1366</v>
+      </c>
+      <c r="K44" s="10">
+        <f t="shared" si="23"/>
+        <v>620</v>
+      </c>
+      <c r="L44" s="10">
+        <f t="shared" si="24"/>
+        <v>266</v>
+      </c>
+      <c r="M44" s="10">
+        <f t="shared" si="25"/>
+        <v>108</v>
+      </c>
+      <c r="N44" s="10">
+        <f t="shared" si="26"/>
+        <v>42</v>
+      </c>
+      <c r="O44" s="10">
+        <f t="shared" si="27"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="10">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10">
+        <f t="shared" si="1"/>
+        <v>991</v>
+      </c>
+      <c r="C45" s="10">
+        <f t="shared" si="2"/>
+        <v>15225</v>
+      </c>
+      <c r="D45" s="10">
+        <f t="shared" si="28"/>
+        <v>28830</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="29"/>
+        <v>16704</v>
+      </c>
+      <c r="F45" s="10">
+        <f t="shared" si="30"/>
+        <v>9504</v>
+      </c>
+      <c r="G45" s="10">
+        <f t="shared" si="21"/>
+        <v>5286</v>
+      </c>
+      <c r="H45" s="10">
+        <f t="shared" si="21"/>
+        <v>2858</v>
+      </c>
+      <c r="I45" s="10">
+        <f t="shared" si="21"/>
+        <v>1492</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="22"/>
+        <v>746</v>
+      </c>
+      <c r="K45" s="10">
+        <f t="shared" si="23"/>
+        <v>354</v>
+      </c>
+      <c r="L45" s="10">
+        <f t="shared" si="24"/>
+        <v>158</v>
+      </c>
+      <c r="M45" s="10">
+        <f t="shared" si="25"/>
+        <v>66</v>
+      </c>
+      <c r="N45" s="10">
+        <f t="shared" si="26"/>
+        <v>26</v>
+      </c>
+      <c r="O45" s="10">
+        <f t="shared" si="27"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="10">
+        <v>45</v>
+      </c>
+      <c r="B46" s="10">
+        <f t="shared" si="1"/>
+        <v>1036</v>
+      </c>
+      <c r="C46" s="10">
+        <f t="shared" si="2"/>
+        <v>16261</v>
+      </c>
+      <c r="D46" s="10">
+        <f t="shared" si="28"/>
+        <v>12126</v>
+      </c>
+      <c r="E46" s="10">
+        <f t="shared" si="29"/>
+        <v>7200</v>
+      </c>
+      <c r="F46" s="10">
+        <f t="shared" si="30"/>
+        <v>4218</v>
+      </c>
+      <c r="G46" s="10">
+        <f t="shared" si="21"/>
+        <v>2428</v>
+      </c>
+      <c r="H46" s="10">
+        <f t="shared" si="21"/>
+        <v>1366</v>
+      </c>
+      <c r="I46" s="10">
+        <f t="shared" si="21"/>
+        <v>746</v>
+      </c>
+      <c r="J46" s="10">
+        <f t="shared" si="22"/>
+        <v>392</v>
+      </c>
+      <c r="K46" s="10">
+        <f t="shared" si="23"/>
+        <v>196</v>
+      </c>
+      <c r="L46" s="10">
+        <f t="shared" si="24"/>
+        <v>92</v>
+      </c>
+      <c r="M46" s="10">
+        <f t="shared" si="25"/>
+        <v>40</v>
+      </c>
+      <c r="N46" s="10">
+        <f t="shared" si="26"/>
+        <v>16</v>
+      </c>
+      <c r="O46" s="10">
+        <f t="shared" si="27"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="10">
+        <v>46</v>
+      </c>
+      <c r="B47" s="10">
+        <f t="shared" si="1"/>
+        <v>1082</v>
+      </c>
+      <c r="C47" s="10">
+        <f t="shared" si="2"/>
+        <v>17343</v>
+      </c>
+      <c r="D47" s="10">
+        <f t="shared" si="28"/>
+        <v>4926</v>
+      </c>
+      <c r="E47" s="10">
+        <f t="shared" si="29"/>
+        <v>2982</v>
+      </c>
+      <c r="F47" s="10">
+        <f t="shared" si="30"/>
+        <v>1790</v>
+      </c>
+      <c r="G47" s="10">
+        <f t="shared" si="21"/>
+        <v>1062</v>
+      </c>
+      <c r="H47" s="10">
+        <f t="shared" si="21"/>
+        <v>620</v>
+      </c>
+      <c r="I47" s="10">
+        <f t="shared" si="21"/>
+        <v>354</v>
+      </c>
+      <c r="J47" s="10">
+        <f t="shared" si="22"/>
+        <v>196</v>
+      </c>
+      <c r="K47" s="10">
+        <f t="shared" si="23"/>
+        <v>104</v>
+      </c>
+      <c r="L47" s="10">
+        <f t="shared" si="24"/>
+        <v>52</v>
+      </c>
+      <c r="M47" s="10">
+        <f t="shared" si="25"/>
+        <v>24</v>
+      </c>
+      <c r="N47" s="10">
+        <f t="shared" si="26"/>
+        <v>10</v>
+      </c>
+      <c r="O47" s="10">
+        <f t="shared" si="27"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="10">
+        <v>47</v>
+      </c>
+      <c r="B48" s="10">
+        <f t="shared" si="1"/>
+        <v>1129</v>
+      </c>
+      <c r="C48" s="10">
+        <f t="shared" si="2"/>
+        <v>18472</v>
+      </c>
+      <c r="D48" s="10">
+        <f t="shared" si="28"/>
+        <v>1944</v>
+      </c>
+      <c r="E48" s="10">
+        <f t="shared" si="29"/>
+        <v>1192</v>
+      </c>
+      <c r="F48" s="10">
+        <f t="shared" si="30"/>
+        <v>728</v>
+      </c>
+      <c r="G48" s="10">
+        <f t="shared" si="21"/>
+        <v>442</v>
+      </c>
+      <c r="H48" s="10">
+        <f t="shared" si="21"/>
+        <v>266</v>
+      </c>
+      <c r="I48" s="10">
+        <f t="shared" si="21"/>
+        <v>158</v>
+      </c>
+      <c r="J48" s="10">
+        <f t="shared" si="22"/>
+        <v>92</v>
+      </c>
+      <c r="K48" s="10">
+        <f t="shared" si="23"/>
+        <v>52</v>
+      </c>
+      <c r="L48" s="10">
+        <f t="shared" si="24"/>
+        <v>28</v>
+      </c>
+      <c r="M48" s="10">
+        <f t="shared" si="25"/>
+        <v>14</v>
+      </c>
+      <c r="N48" s="10">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="O48" s="10">
+        <f t="shared" si="27"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="10">
+        <v>48</v>
+      </c>
+      <c r="B49" s="10">
+        <f t="shared" si="1"/>
+        <v>1177</v>
+      </c>
+      <c r="C49" s="10">
+        <f t="shared" si="2"/>
+        <v>19649</v>
+      </c>
+      <c r="D49" s="10">
+        <f t="shared" si="28"/>
+        <v>752</v>
+      </c>
+      <c r="E49" s="10">
+        <f t="shared" si="29"/>
+        <v>464</v>
+      </c>
+      <c r="F49" s="10">
+        <f t="shared" si="30"/>
+        <v>286</v>
+      </c>
+      <c r="G49" s="10">
+        <f t="shared" ref="G49:L49" si="31">H49+G50</f>
+        <v>176</v>
+      </c>
+      <c r="H49" s="10">
+        <f t="shared" si="31"/>
+        <v>108</v>
+      </c>
+      <c r="I49" s="10">
+        <f t="shared" si="31"/>
+        <v>66</v>
+      </c>
+      <c r="J49" s="10">
+        <f t="shared" si="31"/>
+        <v>40</v>
+      </c>
+      <c r="K49" s="10">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="L49" s="10">
+        <f t="shared" si="31"/>
+        <v>14</v>
+      </c>
+      <c r="M49" s="10">
+        <f>N49+M50</f>
+        <v>8</v>
+      </c>
+      <c r="N49" s="10">
+        <f>N50+N51</f>
+        <v>4</v>
+      </c>
+      <c r="O49" s="10">
+        <f>O50+O51</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="10">
+        <v>49</v>
+      </c>
+      <c r="B50" s="10">
+        <f t="shared" si="1"/>
+        <v>1226</v>
+      </c>
+      <c r="C50" s="10">
+        <f t="shared" si="2"/>
+        <v>20875</v>
+      </c>
+      <c r="D50" s="10">
+        <f t="shared" ref="D50:D51" si="32">E50+F50</f>
+        <v>288</v>
+      </c>
+      <c r="E50" s="10">
+        <f t="shared" ref="E50:E51" si="33">F50+G50</f>
+        <v>178</v>
+      </c>
+      <c r="F50" s="10">
+        <f t="shared" ref="F50:F51" si="34">G50+H50</f>
+        <v>110</v>
+      </c>
+      <c r="G50" s="10">
+        <f t="shared" ref="G50:L50" si="35">H50+I50</f>
+        <v>68</v>
+      </c>
+      <c r="H50" s="10">
+        <f t="shared" si="35"/>
+        <v>42</v>
+      </c>
+      <c r="I50" s="10">
+        <f t="shared" si="35"/>
+        <v>26</v>
+      </c>
+      <c r="J50" s="10">
+        <f t="shared" si="35"/>
+        <v>16</v>
+      </c>
+      <c r="K50" s="10">
+        <f t="shared" si="35"/>
+        <v>10</v>
+      </c>
+      <c r="L50" s="10">
+        <f t="shared" si="35"/>
+        <v>6</v>
+      </c>
+      <c r="M50" s="10">
+        <f>N50+O50</f>
+        <v>4</v>
+      </c>
+      <c r="N50" s="10">
+        <v>2</v>
+      </c>
+      <c r="O50" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="10">
+        <v>50</v>
+      </c>
+      <c r="B51" s="10">
+        <f t="shared" si="1"/>
+        <v>1276</v>
+      </c>
+      <c r="C51" s="10">
+        <f t="shared" si="2"/>
+        <v>22151</v>
+      </c>
+      <c r="D51" s="10">
+        <f t="shared" si="32"/>
+        <v>233</v>
+      </c>
+      <c r="E51" s="10">
+        <f t="shared" si="33"/>
+        <v>144</v>
+      </c>
+      <c r="F51" s="10">
+        <f t="shared" si="34"/>
+        <v>89</v>
+      </c>
+      <c r="G51" s="10">
+        <f t="shared" ref="G51:L51" si="36">H51+I51</f>
+        <v>55</v>
+      </c>
+      <c r="H51" s="10">
+        <f t="shared" si="36"/>
+        <v>34</v>
+      </c>
+      <c r="I51" s="10">
+        <f t="shared" si="36"/>
+        <v>21</v>
+      </c>
+      <c r="J51" s="10">
+        <f t="shared" si="36"/>
+        <v>13</v>
+      </c>
+      <c r="K51" s="10">
+        <f t="shared" si="36"/>
+        <v>8</v>
+      </c>
+      <c r="L51" s="10">
+        <f t="shared" si="36"/>
+        <v>5</v>
+      </c>
+      <c r="M51" s="10">
+        <f>N51+O51</f>
+        <v>3</v>
+      </c>
+      <c r="N51" s="10">
+        <v>2</v>
+      </c>
+      <c r="O51" s="10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added empty cell test
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkennell\Documents\Elixir Projects\xlsx_dir\xlsxir\test\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="4410" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="12795" windowHeight="4410" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +21,7 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
@@ -35,7 +41,7 @@
     <definedName name="_xlnm.Sheet_Title" localSheetId="6">"Sheet7"</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="7">"Sheet8"</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
   <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
@@ -115,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="\_x0009_\ ####.#"/>
     <numFmt numFmtId="165" formatCode="#.0#"/>
@@ -203,6 +209,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -249,7 +263,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,9 +295,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,6 +347,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,7 +540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -529,8 +579,67 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -570,7 +679,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49748,7 +49857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49777,7 +49886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49819,7 +49928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49867,7 +49976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49902,7 +50011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49934,10 +50043,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -50114,51 +50223,51 @@
         <v>14</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D51" si="3">D3+C4</f>
+        <f t="shared" ref="D4:D32" si="3">D3+C4</f>
         <v>25</v>
       </c>
       <c r="E4" s="10">
-        <f t="shared" ref="E4:E51" si="4">E3+D4</f>
+        <f t="shared" ref="E4:E32" si="4">E3+D4</f>
         <v>41</v>
       </c>
       <c r="F4" s="10">
-        <f t="shared" ref="F4:F51" si="5">F3+E4</f>
+        <f t="shared" ref="F4:F32" si="5">F3+E4</f>
         <v>63</v>
       </c>
       <c r="G4" s="10">
-        <f t="shared" ref="G4:G51" si="6">G3+F4</f>
+        <f t="shared" ref="G4:G32" si="6">G3+F4</f>
         <v>92</v>
       </c>
       <c r="H4" s="10">
-        <f t="shared" ref="H4:H51" si="7">H3+G4</f>
+        <f t="shared" ref="H4:H32" si="7">H3+G4</f>
         <v>129</v>
       </c>
       <c r="I4" s="10">
-        <f t="shared" ref="I4:I51" si="8">I3+H4</f>
+        <f t="shared" ref="I4:I26" si="8">I3+H4</f>
         <v>175</v>
       </c>
       <c r="J4" s="10">
-        <f t="shared" ref="J4:J51" si="9">J3+I4</f>
+        <f t="shared" ref="J4:J18" si="9">J3+I4</f>
         <v>231</v>
       </c>
       <c r="K4" s="10">
-        <f t="shared" ref="K4:K51" si="10">K3+J4</f>
+        <f t="shared" ref="K4:K17" si="10">K3+J4</f>
         <v>298</v>
       </c>
       <c r="L4" s="10">
-        <f t="shared" ref="L4:L51" si="11">L3+K4</f>
+        <f t="shared" ref="L4:L17" si="11">L3+K4</f>
         <v>377</v>
       </c>
       <c r="M4" s="10">
-        <f t="shared" ref="M4:M51" si="12">M3+L4</f>
+        <f t="shared" ref="M4:M17" si="12">M3+L4</f>
         <v>469</v>
       </c>
       <c r="N4" s="10">
-        <f t="shared" ref="N4:N51" si="13">N3+M4</f>
+        <f t="shared" ref="N4:N17" si="13">N3+M4</f>
         <v>575</v>
       </c>
       <c r="O4" s="10">
-        <f t="shared" ref="O4:O51" si="14">O3+N4</f>
+        <f t="shared" ref="O4:O17" si="14">O3+N4</f>
         <v>696</v>
       </c>
     </row>
@@ -51092,19 +51201,19 @@
         <v>0.3354166666666667</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" ref="K19:K26" si="16">L20+K21</f>
+        <f t="shared" ref="K20:K26" si="16">L20+K21</f>
         <v>78175076</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" ref="L19:L26" si="17">M20+L21</f>
+        <f t="shared" ref="L20:L26" si="17">M20+L21</f>
         <v>29860634</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" ref="M19:M26" si="18">N20+M21</f>
+        <f t="shared" ref="M20:M26" si="18">N20+M21</f>
         <v>11405772</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" ref="N19:N26" si="19">N21+N22</f>
+        <f t="shared" ref="N20:N26" si="19">N21+N22</f>
         <v>4356618</v>
       </c>
       <c r="O20" s="10">
@@ -51209,7 +51318,7 @@
         <v>11199045</v>
       </c>
       <c r="J22" s="10">
-        <f t="shared" ref="J19:J26" si="20">K22+J23</f>
+        <f t="shared" ref="J22:J26" si="20">K22+J23</f>
         <v>78163168</v>
       </c>
       <c r="K22" s="10">

</xml_diff>

<commit_message>
Ensure value read is from <v/> not <f/> as latter is forumla
This leaves support for returning formula in the cell in the future, but
for now we should mask it so that it would not return the formula if the
calculated value is empty.

Fixes #80
</commit_message>
<xml_diff>
--- a/test/test_data/test.xlsx
+++ b/test/test_data/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkennell\Documents\Elixir Projects\xlsx_dir\xlsxir\test\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenips/Code/github/xlsxir/test/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161E9F75-692B-5C49-9C6A-936B91849CD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="12795" windowHeight="4410" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23060" windowHeight="17060" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +23,7 @@
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
@@ -41,8 +43,15 @@
     <definedName name="_xlnm.Sheet_Title" localSheetId="6">"Sheet7"</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="7">"Sheet8"</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <webPublishing css="0" allowPng="1" codePage="1252"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -121,7 +130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="\_x0009_\ ####.#"/>
     <numFmt numFmtId="165" formatCode="#.0#"/>
@@ -540,14 +549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -580,14 +589,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1">
@@ -631,6 +640,187 @@
       </c>
       <c r="D4">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE18A16-8B80-314A-A6DF-23F022D0F100}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1">
+        <f>IF(Sheet10!A1&lt;&gt;"",Sheet10!A1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="B1" t="str">
+        <f>IF(Sheet10!B1&lt;&gt;"",Sheet10!B1,"")</f>
+        <v/>
+      </c>
+      <c r="C1">
+        <f>IF(Sheet10!C1&lt;&gt;"",Sheet10!C1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="D1" t="str">
+        <f>IF(Sheet10!D1&lt;&gt;"",Sheet10!D1,"")</f>
+        <v/>
+      </c>
+      <c r="E1">
+        <f>IF(Sheet10!E1&lt;&gt;"",Sheet10!E1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="F1" t="str">
+        <f>IF(Sheet10!F1&lt;&gt;"",Sheet10!F1,"")</f>
+        <v/>
+      </c>
+      <c r="G1" t="str">
+        <f>IF(Sheet10!G1&lt;&gt;"",Sheet10!G1,"")</f>
+        <v/>
+      </c>
+      <c r="H1">
+        <f>IF(Sheet10!H1&lt;&gt;"",Sheet10!H1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="I1" t="str">
+        <f>IF(Sheet10!I1&lt;&gt;"",Sheet10!I1,"")</f>
+        <v/>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(Sheet10!J1&lt;&gt;"",Sheet10!J1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="str">
+        <f>IF(Sheet10!A2&lt;&gt;"",Sheet10!A2,"")</f>
+        <v/>
+      </c>
+      <c r="B2">
+        <f>IF(Sheet10!B2&lt;&gt;"",Sheet10!B2,"")</f>
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF(Sheet10!C2&lt;&gt;"",Sheet10!C2,"")</f>
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(Sheet10!D2&lt;&gt;"",Sheet10!D2,"")</f>
+        <v/>
+      </c>
+      <c r="E2">
+        <f>IF(Sheet10!E2&lt;&gt;"",Sheet10!E2,"")</f>
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(Sheet10!F2&lt;&gt;"",Sheet10!F2,"")</f>
+        <v/>
+      </c>
+      <c r="G2">
+        <f>IF(Sheet10!G2&lt;&gt;"",Sheet10!G2,"")</f>
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(Sheet10!H2&lt;&gt;"",Sheet10!H2,"")</f>
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(Sheet10!I2&lt;&gt;"",Sheet10!I2,"")</f>
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(Sheet10!J2&lt;&gt;"",Sheet10!J2,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="str">
+        <f>IF(Sheet10!A3&lt;&gt;"",Sheet10!A3,"")</f>
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <f>IF(Sheet10!B3&lt;&gt;"",Sheet10!B3,"")</f>
+        <v/>
+      </c>
+      <c r="C3" t="str">
+        <f>IF(Sheet10!C3&lt;&gt;"",Sheet10!C3,"")</f>
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(Sheet10!D3&lt;&gt;"",Sheet10!D3,"")</f>
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <f>IF(Sheet10!E3&lt;&gt;"",Sheet10!E3,"")</f>
+        <v/>
+      </c>
+      <c r="F3">
+        <f>IF(Sheet10!F3&lt;&gt;"",Sheet10!F3,"")</f>
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>IF(Sheet10!G3&lt;&gt;"",Sheet10!G3,"")</f>
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <f>IF(Sheet10!H3&lt;&gt;"",Sheet10!H3,"")</f>
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <f>IF(Sheet10!I3&lt;&gt;"",Sheet10!I3,"")</f>
+        <v/>
+      </c>
+      <c r="J3">
+        <f>IF(Sheet10!J3&lt;&gt;"",Sheet10!J3,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <f>IF(Sheet10!A4&lt;&gt;"",Sheet10!A4,"")</f>
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>IF(Sheet10!B4&lt;&gt;"",Sheet10!B4,"")</f>
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IF(Sheet10!C4&lt;&gt;"",Sheet10!C4,"")</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>IF(Sheet10!D4&lt;&gt;"",Sheet10!D4,"")</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <f>IF(Sheet10!E4&lt;&gt;"",Sheet10!E4,"")</f>
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <f>IF(Sheet10!F4&lt;&gt;"",Sheet10!F4,"")</f>
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <f>IF(Sheet10!G4&lt;&gt;"",Sheet10!G4,"")</f>
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <f>IF(Sheet10!H4&lt;&gt;"",Sheet10!H4,"")</f>
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <f>IF(Sheet10!I4&lt;&gt;"",Sheet10!I4,"")</f>
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <f>IF(Sheet10!J4&lt;&gt;"",Sheet10!J4,"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -639,16 +829,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -679,16 +869,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:XFD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -49857,16 +50047,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1048576" sqref="B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1048576" spans="1:1">
@@ -49886,16 +50076,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -49928,20 +50118,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.19921875" style="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.19921875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -49976,17 +50166,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -50011,16 +50201,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -50043,16 +50233,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="14" width="9.140625" style="10"/>
-    <col min="15" max="15" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="14" width="9.19921875" style="10"/>
+    <col min="15" max="15" width="12.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.19921875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">

</xml_diff>